<commit_message>
changed scenario descriptio in Login
</commit_message>
<xml_diff>
--- a/QA/Login.xlsx
+++ b/QA/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\Git\techin-exercises\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E66C30D-C3E2-4247-B7BA-2A1DDF32659D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B688511-5BD9-4F1D-B2F9-C69D0DB0F230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="180" windowWidth="25110" windowHeight="15090" xr2:uid="{CF99234D-968E-4984-8CBB-57F648388ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="76">
   <si>
     <t>TC001</t>
   </si>
@@ -161,9 +161,6 @@
     <t>TS001</t>
   </si>
   <si>
-    <t xml:space="preserve">web page funkcionality </t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
   </si>
   <si>
     <t xml:space="preserve">User must be allready created </t>
-  </si>
-  <si>
-    <t>web page works as intended</t>
   </si>
   <si>
     <t>equivalence partitioning (dif inputs)</t>
@@ -337,6 +331,15 @@
   </si>
   <si>
     <t>No expiration of login session overal</t>
+  </si>
+  <si>
+    <t>Functionality of login function</t>
+  </si>
+  <si>
+    <t>Login function works as intended.</t>
+  </si>
+  <si>
+    <t>TC011</t>
   </si>
 </sst>
 </file>
@@ -888,7 +891,7 @@
   <dimension ref="B2:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,13 +963,13 @@
         <v>35</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
@@ -987,16 +990,16 @@
         <v>9</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" s="13" t="s">
         <v>31</v>
       </c>
       <c r="K5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1023,7 +1026,7 @@
         <v>35</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>9</v>
@@ -1043,7 +1046,7 @@
         <v>35</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>9</v>
@@ -1125,10 +1128,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="8" t="s">
@@ -1143,10 +1146,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="8" t="s">
@@ -1175,10 +1178,10 @@
     <row r="17" spans="2:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="30" x14ac:dyDescent="0.25">
@@ -1250,13 +1253,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>9</v>
@@ -1265,13 +1268,13 @@
         <v>20</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>9</v>
@@ -1297,7 +1300,7 @@
         <v>22</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>24</v>
@@ -1317,7 +1320,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>21</v>
@@ -1345,7 +1348,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>16</v>
@@ -1362,18 +1365,18 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -1389,13 +1392,13 @@
         <v>20</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>9</v>
@@ -1411,13 +1414,13 @@
         <v>22</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>9</v>
@@ -1433,13 +1436,13 @@
         <v>25</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>29</v>
@@ -1450,13 +1453,13 @@
         <v>28</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>29</v>
@@ -1467,13 +1470,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>29</v>
@@ -1481,16 +1484,16 @@
     </row>
     <row r="33" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
@@ -1498,16 +1501,16 @@
     </row>
     <row r="34" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>29</v>
@@ -1515,16 +1518,16 @@
     </row>
     <row r="35" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -1532,31 +1535,33 @@
     </row>
     <row r="36" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="F36" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
-      <c r="C37" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="D37" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>29</v>

</xml_diff>